<commit_message>
rearranged some folders for better readability of this git
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/PythonClassifierApplication_Getr/Ergebnisse_SVM_Getriebe_C.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Getriebe/PythonClassifierApplication_Getr/Ergebnisse_SVM_Getriebe_C.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martinho\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repositories\datascience_sensor_data\Maschinelles_Lernen\PythonClassifierApplication_Getriebe\PythonClassifierApplication_Getr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TPR</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>C-Parameter</t>
+  </si>
+  <si>
+    <t>lineare SVM</t>
   </si>
 </sst>
 </file>
@@ -52,7 +55,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -109,19 +112,19 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -438,161 +441,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0E8F7E-EB4B-4DDE-903A-0584641624B7}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="6" width="13" style="2" customWidth="1"/>
+    <col min="1" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13" style="1" customWidth="1"/>
+    <col min="7" max="10" width="13" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="G2" s="2">
         <v>0.88022670000000003</v>
       </c>
-      <c r="D2" s="2">
+      <c r="H2" s="2">
         <v>0.84523510000000002</v>
       </c>
-      <c r="E2" s="2">
+      <c r="I2" s="2">
         <v>7.93074E-2</v>
       </c>
-      <c r="F2" s="2">
+      <c r="J2" s="2">
         <v>0.1197733</v>
       </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
         <v>1.7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="G3" s="2">
         <v>0.87891859999999999</v>
       </c>
-      <c r="D3" s="2">
+      <c r="H3" s="2">
         <v>0.84280650000000001</v>
       </c>
-      <c r="E3" s="2">
+      <c r="I3" s="2">
         <v>7.8974799999999998E-2</v>
       </c>
-      <c r="F3" s="2">
+      <c r="J3" s="2">
         <v>0.12108140000000001</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
         <v>1.3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="G4" s="2">
         <v>0.87894870000000003</v>
       </c>
-      <c r="D4" s="2">
+      <c r="H4" s="2">
         <v>0.84157590000000004</v>
       </c>
-      <c r="E4" s="2">
+      <c r="I4" s="2">
         <v>7.7508999999999995E-2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="J4" s="2">
         <v>0.1210513</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="4">
+      <c r="G5" s="4">
         <v>0.88004629999999995</v>
       </c>
-      <c r="D5" s="4">
+      <c r="H5" s="4">
         <v>0.84267179999999997</v>
       </c>
-      <c r="E5" s="4">
+      <c r="I5" s="4">
         <v>7.6472600000000002E-2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="J5" s="4">
         <v>0.1199537</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
         <v>0.7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="G6" s="2">
         <v>0.88075289999999995</v>
       </c>
-      <c r="D6" s="2">
+      <c r="H6" s="2">
         <v>0.84575449999999996</v>
       </c>
-      <c r="E6" s="2">
+      <c r="I6" s="2">
         <v>7.8382199999999999E-2</v>
       </c>
-      <c r="F6" s="2">
+      <c r="J6" s="2">
         <v>0.11924700000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
         <v>0.3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="G7" s="2">
         <v>0.88003129999999996</v>
       </c>
-      <c r="D7" s="2">
+      <c r="H7" s="2">
         <v>0.84475679999999997</v>
       </c>
-      <c r="E7" s="2">
+      <c r="I7" s="2">
         <v>7.8873700000000005E-2</v>
       </c>
-      <c r="F7" s="2">
+      <c r="J7" s="2">
         <v>0.1199687</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
         <v>0.01</v>
       </c>
-      <c r="C8" s="2">
+      <c r="G8" s="2">
         <v>0.87983579999999995</v>
       </c>
-      <c r="D8" s="2">
+      <c r="H8" s="2">
         <v>0.84290240000000005</v>
       </c>
-      <c r="E8" s="2">
+      <c r="I8" s="2">
         <v>7.7489000000000002E-2</v>
       </c>
-      <c r="F8" s="2">
+      <c r="J8" s="2">
         <v>0.1201642</v>
       </c>
     </row>

</xml_diff>